<commit_message>
Added credentials check & ask
</commit_message>
<xml_diff>
--- a/TimewaxSync/Planning Timewax.xlsx
+++ b/TimewaxSync/Planning Timewax.xlsx
@@ -1,20 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stesi\source\repos\TimewaxSync\TimewaxSync\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4AD96DD-A1BA-4D83-9D74-C452D55A7C4F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A95395-DE86-455D-8160-4F9CFA058764}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22530" windowHeight="7545" xr2:uid="{0DAB8511-BFE8-4D42-B58F-14807BA41C9A}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{0DAB8511-BFE8-4D42-B58F-14807BA41C9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="Codes">Sheet1!$H:$H</definedName>
+    <definedName name="Dates">Sheet1!$B:$B</definedName>
+    <definedName name="EmployeeCodes">Sheet1!$E:$E</definedName>
+    <definedName name="Employees">Sheet1!$I:$I</definedName>
+    <definedName name="ID">Sheet1!#REF!</definedName>
+    <definedName name="IDs">Sheet1!$A:$A</definedName>
+    <definedName name="Phases">Sheet1!$G:$G</definedName>
+    <definedName name="Projects">Sheet1!$F:$F</definedName>
+    <definedName name="TimeBegin">Sheet1!$C:$C</definedName>
+    <definedName name="TimeEnd">Sheet1!$D:$D</definedName>
+    <definedName name="TimeIDs">Sheet1!$J:$J</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,27 +38,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Datum</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Tijdvan</t>
+  </si>
+  <si>
+    <t>Tijdtot</t>
+  </si>
+  <si>
+    <t>Fase</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Medewerker</t>
+  </si>
+  <si>
+    <t>Tijd-ID</t>
+  </si>
+  <si>
+    <t>MedewekerCode</t>
+  </si>
   <si>
     <t>ID</t>
-  </si>
-  <si>
-    <t>Datum</t>
-  </si>
-  <si>
-    <t>Project</t>
-  </si>
-  <si>
-    <t>Tijdvan</t>
-  </si>
-  <si>
-    <t>Tijdtot</t>
-  </si>
-  <si>
-    <t>Fase</t>
-  </si>
-  <si>
-    <t>Code</t>
   </si>
 </sst>
 </file>
@@ -398,42 +420,53 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A888895-68D9-496E-83BF-D3D8C60AD0C6}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.5703125" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.28515625" customWidth="1"/>
-    <col min="6" max="6" width="39.28515625" customWidth="1"/>
-    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48.28515625" customWidth="1"/>
+    <col min="7" max="7" width="39.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>